<commit_message>
Updated definition of non-empty UtilityNetwork: A UtilityNetwork must contain at least 1 element, ActivityComplex or ProtectedArea
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F01A80-4B4B-4126-AA95-1454EBDA44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57608EA1-66B0-416A-BB2E-B7DA3DA90FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="272">
   <si>
     <t>ElectricityCable</t>
   </si>
@@ -872,54 +872,49 @@
     <t>Strongly recommended to include if an ActivityComplex is present. The referenced ActivityComplex must exist.</t>
   </si>
   <si>
+    <t>Mandatory if there are StandardCoverageDetail objects present that represent the standard coverage for the UtilityNetwork. The referenced StandardCoverageDetail(s) must exist.</t>
+  </si>
+  <si>
+    <t>Mandatory when one or more depth objects are present for any element within the UtilityNetwork. The referenced object(s) must exist.</t>
+  </si>
+  <si>
+    <t>Strict obligation in IMKL. The referenced element(s) must exist.</t>
+  </si>
+  <si>
+    <t>Mandatory when one or more Annotation objects are present. The referenced Annotation(s) must exist.</t>
+  </si>
+  <si>
+    <t>Strongly recommended to include if available. The referenced cable(s) must exist.</t>
+  </si>
+  <si>
+    <t>Strongly recommended to include if available. The referenced pipe(s) must exist.</t>
+  </si>
+  <si>
+    <t>Strongly recommended to include if available. The referenced duct(s) must exist.</t>
+  </si>
+  <si>
+    <t>Recommended to include if applicable. The referenced node(s) must exist.</t>
+  </si>
+  <si>
+    <t>Mandatory when one or more ExtraPlan objects are present. The referenced Document(s) must exist.</t>
+  </si>
+  <si>
+    <t>v4.0</t>
+  </si>
+  <si>
+    <t>Mandatory when one or more elements are present. The referenced element(s) must exist.
+Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex or ProtectedArea.</t>
+  </si>
+  <si>
     <t>Mandatory if one or more ActivityComplex objects are available. The referenced ActivityComplex must exist.
-Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex, ProtectedArea, Document, ExtraPlan or Annotation.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more elements are present. The referenced element(s) must exist.
-Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex, ProtectedArea, Document or Annotation.</t>
+Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex or ProtectedArea</t>
   </si>
   <si>
     <t>Mandatory when one or more ProtectedArea objects are present. The referenced ProtectedArea(s) must exist.
-Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex, ProtectedArea, Document, ExtraPlan or Annotation.</t>
-  </si>
-  <si>
-    <t>Mandatory if there are StandardCoverageDetail objects present that represent the standard coverage for the UtilityNetwork. The referenced StandardCoverageDetail(s) must exist.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more depth objects are present for any element within the UtilityNetwork. The referenced object(s) must exist.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more Annotation objects are present. The referenced Annotation(s) must exist.
-Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex, ProtectedArea, Document, ExtraPlan or Annotation.</t>
-  </si>
-  <si>
-    <t>Strict obligation in IMKL. The referenced element(s) must exist.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more Annotation objects are present. The referenced Annotation(s) must exist.</t>
-  </si>
-  <si>
-    <t>Strongly recommended to include if available. The referenced cable(s) must exist.</t>
-  </si>
-  <si>
-    <t>Strongly recommended to include if available. The referenced pipe(s) must exist.</t>
-  </si>
-  <si>
-    <t>Strongly recommended to include if available. The referenced duct(s) must exist.</t>
-  </si>
-  <si>
-    <t>Recommended to include if applicable. The referenced node(s) must exist.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more ExtraPlan objects are present. The referenced Document(s) must exist.</t>
-  </si>
-  <si>
-    <t>Mandatory when one or more Document or ExtraPlan objects are present. The referenced Document(s) must exist.
-Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex, ProtectedArea, Document, ExtraPlan or Annotation.</t>
-  </si>
-  <si>
-    <t>v4.0</t>
+Empty networks are not allowed. Each network must contain at least 1 element, ActivityComplex or ProtectedArea.</t>
+  </si>
+  <si>
+    <t>Mandatory when one or more Document or ExtraPlan objects are present. The referenced Document(s) must exist.</t>
   </si>
 </sst>
 </file>
@@ -1420,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC605C2-C5D4-4825-9E11-90EE9076291A}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,7 +1437,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -2275,7 +2270,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2295,7 +2290,7 @@
         <v>132</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3128,7 +3123,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3148,7 +3143,7 @@
         <v>132</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3981,7 +3976,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4001,7 +3996,7 @@
         <v>132</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4834,7 +4829,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4854,7 +4849,7 @@
         <v>132</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5287,7 +5282,7 @@
         <v>132</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5307,7 +5302,7 @@
         <v>132</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5327,7 +5322,7 @@
         <v>132</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5687,7 +5682,7 @@
         <v>132</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5707,7 +5702,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6460,7 +6455,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -6480,7 +6475,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -7193,7 +7188,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7213,7 +7208,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7546,7 +7541,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7926,7 +7921,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7946,7 +7941,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8185,7 +8180,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8565,7 +8560,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8585,7 +8580,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8824,7 +8819,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9224,7 +9219,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -9244,7 +9239,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9262,8 +9257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F037272-C335-49D9-940E-9503A9473373}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9326,7 +9321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>31</v>
       </c>
@@ -9343,7 +9338,7 @@
         <v>52</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9386,7 +9381,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
@@ -9403,7 +9398,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9643,7 +9638,7 @@
         <v>52</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9663,10 +9658,10 @@
         <v>52</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>42</v>
       </c>
@@ -9683,10 +9678,10 @@
         <v>52</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>43</v>
       </c>
@@ -9706,7 +9701,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>44</v>
       </c>
@@ -9723,7 +9718,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -9956,7 +9951,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10356,7 +10351,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -10376,7 +10371,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11195,7 +11190,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13812,7 +13807,7 @@
         <v>52</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -14765,7 +14760,7 @@
         <v>52</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -16251,7 +16246,7 @@
         <v>132</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16271,7 +16266,7 @@
         <v>132</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17024,7 +17019,7 @@
         <v>132</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17044,7 +17039,7 @@
         <v>132</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17477,7 +17472,7 @@
         <v>132</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17497,7 +17492,7 @@
         <v>132</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17857,7 +17852,7 @@
         <v>132</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17877,7 +17872,7 @@
         <v>132</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17946,15 +17941,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18214,15 +18200,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18240,4 +18227,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update codelists: add NL labels and fix typos
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A91AA7-A37A-481E-A6FC-7E5357A8BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D868D-5885-47CC-928D-059779F53671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="816" yWindow="2388" windowWidth="34560" windowHeight="22452" firstSheet="13" activeTab="22" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" firstSheet="9" activeTab="20" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -1556,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8BC120-06A7-4659-AA0B-1A9C52390F35}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8AAE2A-CE0F-40D3-BDBB-F982DDEB87C4}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7368,7 +7368,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9305,7 +9305,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10436,8 +10436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9409E086-D93E-407F-8B48-13A80DD3324C}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10557,7 +10557,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10577,7 +10577,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11236,8 +11236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965E3C8A-CCC0-4A57-BA70-5E57D6D07565}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17988,15 +17988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18256,15 +18247,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18282,4 +18274,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change order of endLifespanVersion in documentation for UtilityLinkSets, Annotation and Connection.
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D868D-5885-47CC-928D-059779F53671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF9786C-3FB8-42E0-9532-1D3834AC3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" firstSheet="9" activeTab="20" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" firstSheet="9" activeTab="25" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -1557,7 +1557,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,44 +1620,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2410,7 +2410,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2473,44 +2473,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3262,8 +3262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0553AC-C8D7-405B-BF7B-D5436FA88A29}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3326,44 +3326,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4115,8 +4115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B804D63D-6629-4BE3-A1A2-E77803CCA220}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4179,44 +4179,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4989,7 +4989,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5052,44 +5052,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5802,7 +5802,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5865,44 +5865,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -6534,8 +6534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB1F68D-948C-4BF5-8AE7-6399B7AADE69}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6598,44 +6598,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8006,7 +8006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42D7E87-996B-4413-BBAA-621CDA75E7DB}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -10436,7 +10436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9409E086-D93E-407F-8B48-13A80DD3324C}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
@@ -12207,8 +12207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B0875E-4BBC-4337-B179-D80DFA58D9BF}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15593,7 +15593,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15656,44 +15656,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -16386,7 +16386,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16449,44 +16449,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17158,8 +17158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10379A83-45C8-474C-B01F-0F591E7D96E8}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17222,44 +17222,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17988,6 +17988,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18247,16 +18256,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18274,12 +18282,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add clarification regarding allowed geometry types
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF9786C-3FB8-42E0-9532-1D3834AC3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5492150D-29DD-4A61-86DE-3ED7A6515799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" firstSheet="9" activeTab="25" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
@@ -667,9 +667,6 @@
     <t>referenceSurface &gt; locationSurvey &gt; recordedBy</t>
   </si>
   <si>
-    <t>Must be present if the location of the referenceSurface is different from the location of the element the DepthDetail is linked to.</t>
-  </si>
-  <si>
     <t>No extra rules</t>
   </si>
   <si>
@@ -768,9 +765,6 @@
   <si>
     <t>Strongly recommended when a verticalPosition is used instead of a height or depth if available .
 Additional check on the use of the EPSG:5710 srs and on presence of the srsDimension. The srsDimension must be set to 1.</t>
-  </si>
-  <si>
-    <t>Must be present if the location of the referenceSurface is different from the location of the element the CoverageDetail is linked to.</t>
   </si>
   <si>
     <t>A DepthDetail should have exactly 1 of verticalPosition, height or depth.
@@ -801,10 +795,6 @@
 Geometry must be a valid polygon. Multipolygons are not allowed.</t>
   </si>
   <si>
-    <t>Strict obligation in IMKL. Additional check on the use of Lambert2008 coordinates and on presence of the srsDimension. The srsDimension must be set to 2 or 3.
-Geometry must be a valid point, line, polygon or multipart geometry consisting of points, lines and/or polygons.</t>
-  </si>
-  <si>
     <t>red: obligation/prohibition</t>
   </si>
   <si>
@@ -959,6 +949,19 @@
   <si>
     <t>A StandardCoverageDetail should have exactly 1 of  height or depth.
 The uom must be expressed in either urn:ogc:def:uom:OGC::mm, urn:ogc:def:uom:OGC::cm, urn:ogc:def:uom:OGC::m. Must have a positive value</t>
+  </si>
+  <si>
+    <t>Strict obligation in IMKL. Additional check on the use of Lambert2008 coordinates and on presence of the srsDimension. The srsDimension must be set to 2 or 3.
+Geometry must be a valid point, line, polygon or multipoint, multiline or multipolygon geometry. A combination of geometry types (points, lines and polygons) in a single object is not allowed.</t>
+  </si>
+  <si>
+    <t>Must be present if the location of the referenceSurface is different from the location of the element the DepthDetail is linked to. The location must be a valid point geometry.
+Additional check on the use of Lambert2008 coordinates and on presence of the srsDimension. The srsDimension must be set to 2 or 3.
+Must be a valid point geometry.</t>
+  </si>
+  <si>
+    <t>Must be present if the location of the referenceSurface is different from the location of the element the CoverageDetail is linked to.
+Additional check on the use of Lambert2008 coordinates. Allowed geometry types are: Point and Line</t>
   </si>
 </sst>
 </file>
@@ -1473,38 +1476,38 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -1514,37 +1517,37 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1660,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1757,7 +1760,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1797,7 +1800,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1877,7 +1880,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1897,7 +1900,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2180,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2217,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2237,7 +2240,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2257,7 +2260,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2277,7 +2280,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2297,7 +2300,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2317,7 +2320,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2337,7 +2340,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2377,7 +2380,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2510,7 +2513,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2610,7 +2613,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2650,7 +2653,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2730,7 +2733,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3030,7 +3033,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3070,7 +3073,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3090,7 +3093,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3110,7 +3113,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3130,7 +3133,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3150,7 +3153,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3170,7 +3173,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3190,7 +3193,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3230,7 +3233,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3363,7 +3366,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3463,7 +3466,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3503,7 +3506,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3583,7 +3586,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3648,7 +3651,7 @@
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -3883,7 +3886,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3923,7 +3926,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3943,7 +3946,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3963,7 +3966,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3983,7 +3986,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4003,7 +4006,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4023,7 +4026,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4043,7 +4046,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4083,7 +4086,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4216,7 +4219,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4316,7 +4319,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4356,7 +4359,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4436,7 +4439,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4736,7 +4739,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4776,7 +4779,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4796,7 +4799,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4816,7 +4819,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4836,7 +4839,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4856,7 +4859,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4876,7 +4879,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4896,7 +4899,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4936,7 +4939,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5089,7 +5092,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5189,7 +5192,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5229,7 +5232,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5309,7 +5312,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5329,7 +5332,7 @@
         <v>129</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5349,7 +5352,7 @@
         <v>129</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5369,7 +5372,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5589,7 +5592,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5629,7 +5632,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5649,7 +5652,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5669,7 +5672,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5689,7 +5692,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5709,7 +5712,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5729,7 +5732,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5749,7 +5752,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5789,7 +5792,7 @@
         <v>50</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5802,7 +5805,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5902,7 +5905,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5942,7 +5945,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6082,7 +6085,7 @@
         <v>52</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6202,7 +6205,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -6342,7 +6345,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6382,7 +6385,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6402,7 +6405,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6422,7 +6425,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6442,7 +6445,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6462,7 +6465,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6482,7 +6485,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -6502,7 +6505,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -6522,7 +6525,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -6635,7 +6638,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -6675,7 +6678,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6815,7 +6818,7 @@
         <v>52</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6935,7 +6938,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7075,7 +7078,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7115,7 +7118,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7135,7 +7138,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7155,7 +7158,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7175,7 +7178,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7195,7 +7198,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7215,7 +7218,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7235,7 +7238,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7255,7 +7258,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7368,7 +7371,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7468,7 +7471,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7508,7 +7511,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7548,7 +7551,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7588,7 +7591,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7628,7 +7631,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7688,7 +7691,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7808,7 +7811,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7848,7 +7851,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7868,7 +7871,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7888,7 +7891,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7908,7 +7911,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7928,7 +7931,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7968,7 +7971,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7988,7 +7991,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8107,7 +8110,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8147,7 +8150,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8187,7 +8190,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8227,7 +8230,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8267,7 +8270,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8327,7 +8330,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8447,7 +8450,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8487,7 +8490,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8507,7 +8510,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8527,7 +8530,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8547,7 +8550,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8567,7 +8570,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8607,7 +8610,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8627,7 +8630,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8746,7 +8749,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8786,7 +8789,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8826,7 +8829,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8866,7 +8869,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8886,7 +8889,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8926,7 +8929,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8986,7 +8989,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9106,7 +9109,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9146,7 +9149,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9166,7 +9169,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9186,7 +9189,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9206,7 +9209,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -9226,7 +9229,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9266,7 +9269,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -9286,7 +9289,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9385,7 +9388,7 @@
         <v>52</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9445,7 +9448,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9545,7 +9548,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9645,7 +9648,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9685,7 +9688,7 @@
         <v>52</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9705,7 +9708,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9725,7 +9728,7 @@
         <v>52</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9745,7 +9748,7 @@
         <v>52</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9765,7 +9768,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -9878,7 +9881,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -9918,7 +9921,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9958,7 +9961,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9998,7 +10001,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10018,7 +10021,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10058,7 +10061,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10118,7 +10121,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10238,7 +10241,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10278,7 +10281,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10298,7 +10301,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10318,7 +10321,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10338,7 +10341,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10358,7 +10361,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10398,7 +10401,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -10418,7 +10421,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10537,7 +10540,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10752,7 +10755,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10852,7 +10855,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11012,7 +11015,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11052,7 +11055,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11092,7 +11095,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -11112,7 +11115,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11132,7 +11135,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11152,7 +11155,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -11172,7 +11175,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -11337,7 +11340,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11417,7 +11420,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -11437,7 +11440,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11502,7 +11505,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11602,7 +11605,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11682,7 +11685,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11722,7 +11725,7 @@
         <v>50</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -11782,7 +11785,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -11822,7 +11825,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -11842,7 +11845,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11875,7 +11878,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11975,7 +11978,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12018,7 +12021,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>168</v>
       </c>
@@ -12035,7 +12038,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12075,7 +12078,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -12135,7 +12138,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -12175,7 +12178,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12195,7 +12198,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -12208,7 +12211,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12308,7 +12311,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -12333,10 +12336,10 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>49</v>
@@ -12348,15 +12351,15 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>49</v>
@@ -12373,10 +12376,10 @@
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>49</v>
@@ -12388,15 +12391,15 @@
         <v>50</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>49</v>
@@ -12408,7 +12411,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -12448,7 +12451,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12468,7 +12471,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12488,7 +12491,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -12508,7 +12511,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -12528,7 +12531,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -12661,7 +12664,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -12801,7 +12804,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -12841,7 +12844,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12921,7 +12924,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12961,7 +12964,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12981,7 +12984,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13001,7 +13004,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13021,7 +13024,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13041,7 +13044,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -13094,7 +13097,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13194,7 +13197,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13219,7 +13222,7 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>190</v>
@@ -13254,7 +13257,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13274,7 +13277,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13294,7 +13297,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13334,7 +13337,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13354,7 +13357,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13374,7 +13377,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13394,7 +13397,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13414,10 +13417,10 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>168</v>
       </c>
@@ -13434,7 +13437,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>197</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13454,7 +13457,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13474,7 +13477,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13514,7 +13517,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13534,7 +13537,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13554,7 +13557,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13574,7 +13577,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13594,7 +13597,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13614,7 +13617,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13634,7 +13637,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13654,7 +13657,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13694,7 +13697,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13722,7 +13725,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -13734,7 +13737,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13742,7 +13745,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -13754,7 +13757,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13762,7 +13765,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -13774,7 +13777,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13794,7 +13797,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13814,7 +13817,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13854,7 +13857,7 @@
         <v>52</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -13866,8 +13869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEEBB16-5094-4A68-A615-43B0896E521F}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13967,7 +13970,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13992,7 +13995,7 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>190</v>
@@ -14027,7 +14030,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14047,7 +14050,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14067,7 +14070,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14107,7 +14110,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14127,7 +14130,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14147,7 +14150,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14167,7 +14170,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14187,10 +14190,10 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>168</v>
       </c>
@@ -14207,7 +14210,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>229</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14227,7 +14230,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14247,7 +14250,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14287,7 +14290,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14307,7 +14310,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14327,7 +14330,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14347,7 +14350,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14367,7 +14370,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14387,7 +14390,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14407,7 +14410,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14427,7 +14430,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14467,7 +14470,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14495,7 +14498,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -14507,7 +14510,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14515,7 +14518,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -14527,7 +14530,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14535,7 +14538,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -14547,7 +14550,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14567,7 +14570,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14587,7 +14590,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14607,7 +14610,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14647,7 +14650,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14675,7 +14678,7 @@
         <v>63</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>59</v>
@@ -14687,7 +14690,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14695,7 +14698,7 @@
         <v>64</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>59</v>
@@ -14707,7 +14710,7 @@
         <v>50</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14715,7 +14718,7 @@
         <v>65</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>59</v>
@@ -14727,7 +14730,7 @@
         <v>50</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14747,7 +14750,7 @@
         <v>50</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14767,7 +14770,7 @@
         <v>50</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14807,7 +14810,7 @@
         <v>52</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -14920,7 +14923,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14945,7 +14948,7 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>190</v>
@@ -14980,7 +14983,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15000,7 +15003,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15020,7 +15023,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15060,7 +15063,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15080,7 +15083,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15100,7 +15103,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15120,7 +15123,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15140,7 +15143,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15160,7 +15163,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15180,7 +15183,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15200,7 +15203,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15240,7 +15243,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15260,7 +15263,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15280,7 +15283,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15300,7 +15303,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15320,7 +15323,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15340,7 +15343,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15360,7 +15363,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15380,7 +15383,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15420,7 +15423,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15448,7 +15451,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -15460,7 +15463,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15468,7 +15471,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -15480,7 +15483,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15488,7 +15491,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -15500,7 +15503,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15520,7 +15523,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15540,7 +15543,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15560,7 +15563,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15693,7 +15696,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15793,7 +15796,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15833,7 +15836,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16153,7 +16156,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16193,7 +16196,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16213,7 +16216,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16233,7 +16236,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16253,7 +16256,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -16273,7 +16276,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16293,7 +16296,7 @@
         <v>129</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16313,7 +16316,7 @@
         <v>129</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -16353,7 +16356,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16373,7 +16376,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -16486,7 +16489,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -16586,7 +16589,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16626,7 +16629,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16926,7 +16929,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16966,7 +16969,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16986,7 +16989,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17006,7 +17009,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17026,7 +17029,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -17046,7 +17049,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17066,7 +17069,7 @@
         <v>129</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17086,7 +17089,7 @@
         <v>129</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17126,7 +17129,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -17146,7 +17149,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -17259,7 +17262,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17359,7 +17362,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17399,7 +17402,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17479,7 +17482,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17499,7 +17502,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17519,7 +17522,7 @@
         <v>129</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17539,7 +17542,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17759,7 +17762,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17799,7 +17802,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17819,7 +17822,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17839,7 +17842,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17859,7 +17862,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -17879,7 +17882,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17899,7 +17902,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17919,7 +17922,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17959,7 +17962,7 @@
         <v>50</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17979,7 +17982,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -17988,15 +17991,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18256,15 +18250,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18282,4 +18277,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated namespace for UtilityLink references
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADAD5AB-41F3-4488-B8B3-F827934CA1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37663FCD-997A-486A-8F2E-3A4075D6BDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" firstSheet="9" activeTab="21" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="7908" yWindow="2052" windowWidth="34560" windowHeight="22452" firstSheet="13" activeTab="22" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="282">
   <si>
     <t>ElectricityCable</t>
   </si>
@@ -959,6 +959,9 @@
   <si>
     <t>Must be present if the location of the referenceSurface is different from the location of the element the CoverageDetail is linked to.
 Additional check on the use of Lambert2008 coordinates. Allowed geometry types are: Point and Line</t>
+  </si>
+  <si>
+    <t>cdata tags are not allowed. Is not visible in the viewer.</t>
   </si>
 </sst>
 </file>
@@ -10751,7 +10754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97D51E3-6157-4789-B11D-E5D0ED63B0B3}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -11236,8 +11239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965E3C8A-CCC0-4A57-BA70-5E57D6D07565}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11377,7 +11380,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>96</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17988,15 +17991,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18256,15 +18250,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18282,4 +18277,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Replace // with /
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_ExtraRules.xlsx
+++ b/implementation/Documentation/IMKL3_ExtraRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37663FCD-997A-486A-8F2E-3A4075D6BDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B04C98-A5F4-491D-BB13-B0C0F55B9E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7908" yWindow="2052" windowWidth="34560" windowHeight="22452" firstSheet="13" activeTab="22" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
+    <workbookView xWindow="10656" yWindow="6288" windowWidth="34560" windowHeight="22452" firstSheet="13" activeTab="24" xr2:uid="{9D17743D-328E-4A6F-BE90-89AFCBF75199}"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL3 Extra Rules" sheetId="1" r:id="rId1"/>
@@ -607,9 +607,6 @@
     <t>protectedAreaType</t>
   </si>
   <si>
-    <t>cdata tags are not allowed. Is not visible in the viewer if included.</t>
-  </si>
-  <si>
     <t>function</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>cdata tags are not allowed. Is not visible in the viewer.</t>
+  </si>
+  <si>
+    <t>No extra rules. Is visible in the viewer.</t>
   </si>
 </sst>
 </file>
@@ -1476,38 +1476,38 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -1517,37 +1517,37 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1660,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1760,7 +1760,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1800,7 +1800,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1880,7 +1880,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2180,7 +2180,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2220,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2240,7 +2240,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2260,7 +2260,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2280,7 +2280,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2300,7 +2300,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2320,7 +2320,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2340,7 +2340,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2380,7 +2380,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2513,7 +2513,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2613,7 +2613,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2653,7 +2653,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2733,7 +2733,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3033,7 +3033,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3073,7 +3073,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3093,7 +3093,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3113,7 +3113,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3133,7 +3133,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3173,7 +3173,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3193,7 +3193,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3233,7 +3233,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3366,7 +3366,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3466,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3506,7 +3506,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3586,7 +3586,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3651,7 +3651,7 @@
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -3886,7 +3886,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3926,7 +3926,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3946,7 +3946,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3966,7 +3966,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3986,7 +3986,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4006,7 +4006,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4026,7 +4026,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4046,7 +4046,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4219,7 +4219,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4319,7 +4319,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4359,7 +4359,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4439,7 +4439,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4739,7 +4739,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4779,7 +4779,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4799,7 +4799,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4819,7 +4819,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -4839,7 +4839,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4859,7 +4859,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4879,7 +4879,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -4899,7 +4899,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4939,7 +4939,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -4992,7 +4992,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5092,7 +5092,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5192,7 +5192,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5232,7 +5232,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5312,7 +5312,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5332,7 +5332,7 @@
         <v>129</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5352,7 +5352,7 @@
         <v>129</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5372,7 +5372,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5592,7 +5592,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5632,7 +5632,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5652,7 +5652,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5672,7 +5672,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5692,7 +5692,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5712,7 +5712,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5732,7 +5732,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5752,7 +5752,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5792,7 +5792,7 @@
         <v>50</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5905,7 +5905,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5945,7 +5945,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6085,7 +6085,7 @@
         <v>52</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6205,7 +6205,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -6345,7 +6345,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6385,7 +6385,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6405,7 +6405,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6425,7 +6425,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6445,7 +6445,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6465,7 +6465,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6485,7 +6485,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -6505,7 +6505,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -6525,7 +6525,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -6638,7 +6638,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -6678,7 +6678,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6818,7 +6818,7 @@
         <v>52</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6938,7 +6938,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7078,7 +7078,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7118,7 +7118,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7138,7 +7138,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7158,7 +7158,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7178,7 +7178,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7198,7 +7198,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7218,7 +7218,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7238,7 +7238,7 @@
         <v>52</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7258,7 +7258,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7471,7 +7471,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7511,7 +7511,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7551,7 +7551,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7591,7 +7591,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7631,7 +7631,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7691,7 +7691,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7811,7 +7811,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7851,7 +7851,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7871,7 +7871,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7891,7 +7891,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -7911,7 +7911,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -7931,7 +7931,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7971,7 +7971,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7991,7 +7991,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8110,7 +8110,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8150,7 +8150,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8190,7 +8190,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8230,7 +8230,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8270,7 +8270,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8330,7 +8330,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8450,7 +8450,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8490,7 +8490,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8510,7 +8510,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8530,7 +8530,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8550,7 +8550,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8570,7 +8570,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8610,7 +8610,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8630,7 +8630,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8749,7 +8749,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -8789,7 +8789,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8829,7 +8829,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8869,7 +8869,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8889,7 +8889,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -8929,7 +8929,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -8989,7 +8989,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9109,7 +9109,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9149,7 +9149,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9169,7 +9169,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9189,7 +9189,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9209,7 +9209,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -9229,7 +9229,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9269,7 +9269,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -9289,7 +9289,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9388,7 +9388,7 @@
         <v>52</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9448,7 +9448,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9548,7 +9548,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9648,7 +9648,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -9688,7 +9688,7 @@
         <v>52</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9708,7 +9708,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9728,7 +9728,7 @@
         <v>52</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9748,7 +9748,7 @@
         <v>52</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -9768,7 +9768,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -9881,7 +9881,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -9921,7 +9921,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -9961,7 +9961,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10001,7 +10001,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10021,7 +10021,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10061,7 +10061,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10121,7 +10121,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10241,7 +10241,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10281,7 +10281,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10301,7 +10301,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10321,7 +10321,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10341,7 +10341,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10361,7 +10361,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -10401,7 +10401,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -10421,7 +10421,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="4:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10540,7 +10540,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -10855,7 +10855,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11015,7 +11015,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11055,7 +11055,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11095,7 +11095,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -11115,7 +11115,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11135,7 +11135,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11155,7 +11155,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -11175,7 +11175,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -11239,7 +11239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965E3C8A-CCC0-4A57-BA70-5E57D6D07565}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -11340,7 +11340,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11380,7 +11380,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11420,7 +11420,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -11440,7 +11440,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11605,7 +11605,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11685,7 +11685,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11725,7 +11725,7 @@
         <v>50</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -11785,7 +11785,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -11825,7 +11825,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -11845,7 +11845,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11877,8 +11877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52607BE3-DC00-46A5-B151-3ABD17EEE6D5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11978,7 +11978,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -11998,7 +11998,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>92</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12018,7 +12018,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>177</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -12038,7 +12038,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12078,7 +12078,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -12138,7 +12138,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -12178,7 +12178,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12198,7 +12198,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -12311,7 +12311,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -12336,10 +12336,10 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>49</v>
@@ -12351,15 +12351,15 @@
         <v>50</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>49</v>
@@ -12376,10 +12376,10 @@
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>49</v>
@@ -12391,15 +12391,15 @@
         <v>50</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>49</v>
@@ -12411,7 +12411,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -12451,7 +12451,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12471,7 +12471,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12491,7 +12491,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -12511,7 +12511,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -12531,7 +12531,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -12595,7 +12595,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -12609,13 +12609,13 @@
     </row>
     <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>45</v>
@@ -12635,7 +12635,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>46</v>
@@ -12644,7 +12644,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12655,7 +12655,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -12664,18 +12664,18 @@
         <v>50</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>55</v>
@@ -12689,13 +12689,13 @@
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>55</v>
@@ -12704,18 +12704,18 @@
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>45</v>
@@ -12729,13 +12729,13 @@
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>45</v>
@@ -12752,10 +12752,10 @@
         <v>39</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>46</v>
@@ -12775,7 +12775,7 @@
         <v>66</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D12" s="10">
         <v>1</v>
@@ -12784,7 +12784,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12795,7 +12795,7 @@
         <v>66</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>46</v>
@@ -12804,7 +12804,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -12815,7 +12815,7 @@
         <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -12835,7 +12835,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>46</v>
@@ -12844,7 +12844,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12924,7 +12924,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12964,7 +12964,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -12984,7 +12984,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13004,7 +13004,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13024,7 +13024,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13044,12 +13044,12 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>66</v>
@@ -13064,7 +13064,7 @@
         <v>52</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13197,12 +13197,12 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>66</v>
@@ -13222,10 +13222,10 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -13245,7 +13245,7 @@
         <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>59</v>
@@ -13257,15 +13257,15 @@
         <v>50</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>59</v>
@@ -13277,7 +13277,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13285,7 +13285,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>59</v>
@@ -13297,7 +13297,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13305,7 +13305,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -13325,7 +13325,7 @@
         <v>63</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>59</v>
@@ -13337,7 +13337,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13345,7 +13345,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>59</v>
@@ -13357,7 +13357,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13365,7 +13365,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>59</v>
@@ -13377,7 +13377,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13385,7 +13385,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>59</v>
@@ -13397,7 +13397,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13405,7 +13405,7 @@
         <v>103</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>59</v>
@@ -13417,7 +13417,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -13425,7 +13425,7 @@
         <v>168</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>59</v>
@@ -13437,7 +13437,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13445,7 +13445,7 @@
         <v>124</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>59</v>
@@ -13457,7 +13457,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13465,7 +13465,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>59</v>
@@ -13477,7 +13477,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13485,7 +13485,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>59</v>
@@ -13505,7 +13505,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>59</v>
@@ -13517,7 +13517,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13525,7 +13525,7 @@
         <v>64</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>59</v>
@@ -13537,7 +13537,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13545,7 +13545,7 @@
         <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>59</v>
@@ -13557,7 +13557,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13565,7 +13565,7 @@
         <v>102</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>59</v>
@@ -13577,7 +13577,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13585,7 +13585,7 @@
         <v>103</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>59</v>
@@ -13597,7 +13597,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13617,7 +13617,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13637,12 +13637,12 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>66</v>
@@ -13657,12 +13657,12 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>66</v>
@@ -13685,7 +13685,7 @@
         <v>100</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>59</v>
@@ -13697,7 +13697,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13705,7 +13705,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>59</v>
@@ -13725,7 +13725,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -13737,7 +13737,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13745,7 +13745,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -13757,7 +13757,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -13765,7 +13765,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -13777,7 +13777,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13785,7 +13785,7 @@
         <v>102</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>59</v>
@@ -13797,7 +13797,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13805,7 +13805,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>59</v>
@@ -13817,7 +13817,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13842,7 +13842,7 @@
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>66</v>
@@ -13857,7 +13857,7 @@
         <v>52</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -13970,12 +13970,12 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>66</v>
@@ -13995,10 +13995,10 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -14018,7 +14018,7 @@
         <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>59</v>
@@ -14030,15 +14030,15 @@
         <v>50</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>59</v>
@@ -14050,7 +14050,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14058,7 +14058,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>59</v>
@@ -14070,7 +14070,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14078,7 +14078,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -14098,7 +14098,7 @@
         <v>63</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>59</v>
@@ -14110,7 +14110,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14118,7 +14118,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>59</v>
@@ -14130,7 +14130,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14138,7 +14138,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>59</v>
@@ -14150,7 +14150,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14158,7 +14158,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>59</v>
@@ -14170,7 +14170,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14178,7 +14178,7 @@
         <v>103</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>59</v>
@@ -14190,7 +14190,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14198,7 +14198,7 @@
         <v>168</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>59</v>
@@ -14210,7 +14210,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14218,7 +14218,7 @@
         <v>124</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>59</v>
@@ -14230,7 +14230,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14238,7 +14238,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>59</v>
@@ -14250,7 +14250,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14258,7 +14258,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>59</v>
@@ -14278,7 +14278,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>59</v>
@@ -14290,7 +14290,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14298,7 +14298,7 @@
         <v>64</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>59</v>
@@ -14310,7 +14310,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14318,7 +14318,7 @@
         <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>59</v>
@@ -14330,7 +14330,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14338,7 +14338,7 @@
         <v>102</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>59</v>
@@ -14350,7 +14350,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14358,7 +14358,7 @@
         <v>103</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>59</v>
@@ -14370,7 +14370,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14390,7 +14390,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14410,12 +14410,12 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>66</v>
@@ -14430,12 +14430,12 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>66</v>
@@ -14458,7 +14458,7 @@
         <v>100</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>59</v>
@@ -14470,7 +14470,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14478,7 +14478,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>59</v>
@@ -14498,7 +14498,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -14510,7 +14510,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14518,7 +14518,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -14530,7 +14530,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14538,7 +14538,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -14550,7 +14550,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14558,7 +14558,7 @@
         <v>102</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>59</v>
@@ -14570,7 +14570,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14578,7 +14578,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>59</v>
@@ -14590,7 +14590,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14610,7 +14610,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14650,7 +14650,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14678,7 +14678,7 @@
         <v>63</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>59</v>
@@ -14690,7 +14690,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14698,7 +14698,7 @@
         <v>64</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>59</v>
@@ -14710,7 +14710,7 @@
         <v>50</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14718,7 +14718,7 @@
         <v>65</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>59</v>
@@ -14730,7 +14730,7 @@
         <v>50</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -14750,7 +14750,7 @@
         <v>50</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14770,7 +14770,7 @@
         <v>50</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -14795,7 +14795,7 @@
     </row>
     <row r="47" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>66</v>
@@ -14810,7 +14810,7 @@
         <v>52</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -14923,12 +14923,12 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>66</v>
@@ -14948,10 +14948,10 @@
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -14971,7 +14971,7 @@
         <v>74</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>59</v>
@@ -14983,15 +14983,15 @@
         <v>50</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>59</v>
@@ -15003,7 +15003,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15011,7 +15011,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>59</v>
@@ -15023,7 +15023,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15031,7 +15031,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -15051,7 +15051,7 @@
         <v>63</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>59</v>
@@ -15063,7 +15063,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15071,7 +15071,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>59</v>
@@ -15083,7 +15083,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15091,7 +15091,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>59</v>
@@ -15103,7 +15103,7 @@
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15111,7 +15111,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>59</v>
@@ -15123,7 +15123,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15131,7 +15131,7 @@
         <v>103</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>59</v>
@@ -15143,7 +15143,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15151,7 +15151,7 @@
         <v>168</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>59</v>
@@ -15163,7 +15163,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15171,7 +15171,7 @@
         <v>124</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>59</v>
@@ -15183,7 +15183,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15191,7 +15191,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>59</v>
@@ -15203,7 +15203,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15211,7 +15211,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>59</v>
@@ -15231,7 +15231,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>59</v>
@@ -15243,7 +15243,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15251,7 +15251,7 @@
         <v>64</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>59</v>
@@ -15263,7 +15263,7 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15271,7 +15271,7 @@
         <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>59</v>
@@ -15283,7 +15283,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15291,7 +15291,7 @@
         <v>102</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>59</v>
@@ -15303,7 +15303,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15311,7 +15311,7 @@
         <v>103</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>59</v>
@@ -15323,7 +15323,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15343,7 +15343,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15363,12 +15363,12 @@
         <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>66</v>
@@ -15383,12 +15383,12 @@
         <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>66</v>
@@ -15411,7 +15411,7 @@
         <v>100</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>59</v>
@@ -15423,7 +15423,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15431,7 +15431,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>59</v>
@@ -15451,7 +15451,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>59</v>
@@ -15463,7 +15463,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15471,7 +15471,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>59</v>
@@ -15483,7 +15483,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -15491,7 +15491,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>59</v>
@@ -15503,7 +15503,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15511,7 +15511,7 @@
         <v>102</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>59</v>
@@ -15523,7 +15523,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15531,7 +15531,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>59</v>
@@ -15543,7 +15543,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15563,7 +15563,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15696,7 +15696,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -15796,7 +15796,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -15836,7 +15836,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16156,7 +16156,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16196,7 +16196,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16216,7 +16216,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16236,7 +16236,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16256,7 +16256,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -16276,7 +16276,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16296,7 +16296,7 @@
         <v>129</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16316,7 +16316,7 @@
         <v>129</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -16356,7 +16356,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16376,7 +16376,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -16389,7 +16389,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16489,7 +16489,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -16589,7 +16589,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16629,7 +16629,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16929,7 +16929,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16969,7 +16969,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -16989,7 +16989,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17009,7 +17009,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17029,7 +17029,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -17049,7 +17049,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17069,7 +17069,7 @@
         <v>129</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17089,7 +17089,7 @@
         <v>129</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17129,7 +17129,7 @@
         <v>50</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -17149,7 +17149,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -17262,7 +17262,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17362,7 +17362,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17402,7 +17402,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17482,7 +17482,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17502,7 +17502,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17522,7 +17522,7 @@
         <v>129</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17542,7 +17542,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17762,7 +17762,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17802,7 +17802,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17822,7 +17822,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17842,7 +17842,7 @@
         <v>50</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17862,7 +17862,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -17882,7 +17882,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17902,7 +17902,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17922,7 +17922,7 @@
         <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -17962,7 +17962,7 @@
         <v>50</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -17982,7 +17982,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -17991,6 +17991,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -18250,16 +18259,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDFEA48-FAC4-456B-938A-80A9A9627A87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18277,12 +18285,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B8F187-0BAA-4690-94B5-13DD63965D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>